<commit_message>
working on spreadsheet to read into r
</commit_message>
<xml_diff>
--- a/ProcessedData/ArcPro_export/edit/gavi-trib3_XWD_export_eledata_EDIT.xlsx
+++ b/ProcessedData/ArcPro_export/edit/gavi-trib3_XWD_export_eledata_EDIT.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://adminliveunc-my.sharepoint.com/personal/kriddie_ad_unc_edu/Documents/Documents/Ecuador2021/ProcessedData/ArcPro_export/edit/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kriddie/Documents/Ecuador2021/ProcessedData/ArcPro_export/edit/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="36" documentId="8_{CEFD6B0C-72E5-4ED1-AC0B-0434C7F1A475}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9C3F5CDD-8B55-434C-89A2-278EFAA2760D}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EB1A5A7-63D2-574B-B6D0-5BA9321549D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2520" yWindow="705" windowWidth="22110" windowHeight="14625" xr2:uid="{C5667C3A-32A2-471C-845C-E5773241FE5B}"/>
+    <workbookView xWindow="200" yWindow="5680" windowWidth="22120" windowHeight="14620" xr2:uid="{C5667C3A-32A2-471C-845C-E5773241FE5B}"/>
   </bookViews>
   <sheets>
     <sheet name="Gavitrib3_dmt_extractvalues" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029" calcOnSave="0"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="22">
   <si>
     <t>lat_fit</t>
   </si>
@@ -65,40 +66,10 @@
     <t>notes</t>
   </si>
   <si>
-    <t>3.5</t>
-  </si>
-  <si>
-    <t>10</t>
-  </si>
-  <si>
-    <t>2.5</t>
-  </si>
-  <si>
-    <t>18</t>
-  </si>
-  <si>
     <t>NA</t>
   </si>
   <si>
-    <t>20</t>
-  </si>
-  <si>
-    <t>21</t>
-  </si>
-  <si>
-    <t>29</t>
-  </si>
-  <si>
     <t>underground</t>
-  </si>
-  <si>
-    <t>31</t>
-  </si>
-  <si>
-    <t>40</t>
-  </si>
-  <si>
-    <t>50</t>
   </si>
   <si>
     <t>ele_arcpro</t>
@@ -145,12 +116,12 @@
       <b/>
       <sz val="10"/>
       <name val="Arial"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -183,7 +154,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
@@ -191,6 +162,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -206,10 +180,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -536,19 +506,19 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E14" sqref="E14"/>
+      <selection pane="bottomLeft" activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="4" width="16" customWidth="1"/>
-    <col min="5" max="9" width="20.85546875" customWidth="1"/>
-    <col min="10" max="14" width="18.42578125" customWidth="1"/>
+    <col min="5" max="9" width="20.83203125" customWidth="1"/>
+    <col min="10" max="14" width="18.5" customWidth="1"/>
     <col min="15" max="15" width="50" customWidth="1"/>
     <col min="16" max="16" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -571,7 +541,7 @@
         <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>7</v>
@@ -580,31 +550,31 @@
         <v>8</v>
       </c>
       <c r="K1" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="L1" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="M1" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="N1" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="O1" s="1" t="s">
         <v>9</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A2" s="2">
         <v>-0.32709963902289901</v>
       </c>
@@ -617,21 +587,21 @@
       <c r="D2" s="2">
         <v>8.9208666246115396</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>13</v>
+      <c r="E2" s="6">
+        <v>10</v>
+      </c>
+      <c r="F2" s="6">
+        <v>2.5</v>
+      </c>
+      <c r="G2" s="6">
+        <v>18</v>
       </c>
       <c r="H2" s="2"/>
       <c r="I2" s="2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="K2" s="2"/>
       <c r="L2" s="2"/>
@@ -650,7 +620,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A3" s="2">
         <v>-0.32716623902289899</v>
       </c>
@@ -663,21 +633,21 @@
       <c r="D3" s="2">
         <v>17.8417332492231</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>16</v>
+      <c r="E3" s="6">
+        <v>20</v>
+      </c>
+      <c r="F3" s="6">
+        <v>3.5</v>
+      </c>
+      <c r="G3" s="6">
+        <v>21</v>
       </c>
       <c r="H3" s="2"/>
       <c r="I3" s="2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="K3" s="2"/>
       <c r="L3" s="2"/>
@@ -696,7 +666,7 @@
         <v>5.6569009346003438E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A4" s="2">
         <v>-0.32729353902289898</v>
       </c>
@@ -709,21 +679,21 @@
       <c r="D4" s="2">
         <v>35.683466498446201</v>
       </c>
-      <c r="E4" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>15</v>
+      <c r="E4" s="6">
+        <v>40</v>
+      </c>
+      <c r="F4" s="6">
+        <v>3.5</v>
+      </c>
+      <c r="G4" s="6">
+        <v>20</v>
       </c>
       <c r="H4" s="2"/>
       <c r="I4" s="2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
@@ -734,7 +704,7 @@
         <v>4105.19091796875</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A5" s="3">
         <v>-0.327226739022899</v>
       </c>
@@ -747,34 +717,34 @@
       <c r="D5" s="3">
         <v>25.870513211373499</v>
       </c>
-      <c r="E5" s="3" t="s">
-        <v>17</v>
+      <c r="E5" s="7">
+        <v>29</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="H5" s="3"/>
       <c r="I5" s="3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="K5" s="3"/>
       <c r="L5" s="3"/>
       <c r="M5" s="3"/>
       <c r="N5" s="3"/>
       <c r="O5" s="3" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="P5" s="3">
         <v>4106.109375</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A6" s="3">
         <v>-0.32723973902289899</v>
       </c>
@@ -787,34 +757,34 @@
       <c r="D6" s="3">
         <v>27.654686536295799</v>
       </c>
-      <c r="E6" s="3" t="s">
-        <v>19</v>
+      <c r="E6" s="7">
+        <v>31</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="H6" s="3"/>
       <c r="I6" s="3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="K6" s="3"/>
       <c r="L6" s="3"/>
       <c r="M6" s="3"/>
       <c r="N6" s="3"/>
       <c r="O6" s="3" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="P6" s="3">
         <v>4105.8173828125</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A7" s="3">
         <v>-0.32734363902289898</v>
       </c>
@@ -827,21 +797,21 @@
       <c r="D7" s="3">
         <v>44.6043331230577</v>
       </c>
-      <c r="E7" s="3" t="s">
-        <v>21</v>
+      <c r="E7" s="7">
+        <v>50</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="H7" s="3"/>
       <c r="I7" s="3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="K7" s="3"/>
       <c r="L7" s="3"/>
@@ -852,7 +822,7 @@
         <v>4104.736328125</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>-0.32733903902289901</v>
       </c>
@@ -881,13 +851,13 @@
         <v>627.08240000000001</v>
       </c>
       <c r="M8" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="N8" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>-0.32722793902289898</v>
       </c>
@@ -916,13 +886,13 @@
         <v>626.23339999999996</v>
       </c>
       <c r="M9" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="N9" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A10">
         <v>-0.32717543902289897</v>
       </c>
@@ -951,13 +921,13 @@
         <v>626.18640000000005</v>
       </c>
       <c r="M10" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="N10" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>-0.32711823902289899</v>
       </c>
@@ -986,13 +956,13 @@
         <v>627.11239999999998</v>
       </c>
       <c r="M11" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="N11" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A12">
         <v>-0.32711163902289903</v>
       </c>
@@ -1021,13 +991,13 @@
         <v>626.09040000000005</v>
       </c>
       <c r="M12" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="N12" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>-0.32704063902289898</v>
       </c>
@@ -1056,13 +1026,13 @@
         <v>627.14239999999995</v>
       </c>
       <c r="M13" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="N13" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>-0.32704063902289898</v>
       </c>
@@ -1091,10 +1061,10 @@
         <v>626.14739999999995</v>
       </c>
       <c r="M14" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="N14" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -1106,4 +1076,539 @@
     <oddFooter>&amp;F</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49C6DD98-9AA2-2046-9454-4B9629CDA1E3}">
+  <dimension ref="A1:R14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="8" max="8" width="7.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" t="s">
+        <v>16</v>
+      </c>
+      <c r="L1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M1" t="s">
+        <v>18</v>
+      </c>
+      <c r="N1" t="s">
+        <v>19</v>
+      </c>
+      <c r="O1" t="s">
+        <v>9</v>
+      </c>
+      <c r="P1" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>13</v>
+      </c>
+      <c r="R1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A2">
+        <v>-0.32709963902289901</v>
+      </c>
+      <c r="B2">
+        <v>-78.200967619395101</v>
+      </c>
+      <c r="C2">
+        <v>4110.4050187176799</v>
+      </c>
+      <c r="D2">
+        <v>8.9208666246115396</v>
+      </c>
+      <c r="E2" s="5">
+        <v>10</v>
+      </c>
+      <c r="F2" s="5">
+        <v>2.5</v>
+      </c>
+      <c r="G2" s="5">
+        <v>18</v>
+      </c>
+      <c r="H2" s="2"/>
+      <c r="I2" t="s">
+        <v>10</v>
+      </c>
+      <c r="J2" t="s">
+        <v>10</v>
+      </c>
+      <c r="P2">
+        <v>4108.1640625</v>
+      </c>
+      <c r="Q2" t="e">
+        <v>#REF!</v>
+      </c>
+      <c r="R2" t="e">
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A3">
+        <v>-0.32716623902289899</v>
+      </c>
+      <c r="B3">
+        <v>-78.200922986052305</v>
+      </c>
+      <c r="C3">
+        <v>4109.8037201468796</v>
+      </c>
+      <c r="D3">
+        <v>17.8417332492231</v>
+      </c>
+      <c r="E3" s="5">
+        <v>20</v>
+      </c>
+      <c r="F3" s="5">
+        <v>3.5</v>
+      </c>
+      <c r="G3" s="5">
+        <v>21</v>
+      </c>
+      <c r="H3" s="2"/>
+      <c r="I3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J3" t="s">
+        <v>10</v>
+      </c>
+      <c r="P3">
+        <v>4106.96533203125</v>
+      </c>
+      <c r="Q3">
+        <v>30</v>
+      </c>
+      <c r="R3">
+        <v>5.6569009346003438E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A4">
+        <v>-0.32729353902289898</v>
+      </c>
+      <c r="B4">
+        <v>-78.200826563555793</v>
+      </c>
+      <c r="C4">
+        <v>4108.7079484372998</v>
+      </c>
+      <c r="D4">
+        <v>35.683466498446201</v>
+      </c>
+      <c r="E4" s="5">
+        <v>40</v>
+      </c>
+      <c r="F4" s="5">
+        <v>3.5</v>
+      </c>
+      <c r="G4" s="5">
+        <v>20</v>
+      </c>
+      <c r="H4" s="2"/>
+      <c r="I4" t="s">
+        <v>10</v>
+      </c>
+      <c r="J4" t="s">
+        <v>10</v>
+      </c>
+      <c r="P4">
+        <v>4105.19091796875</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A5">
+        <v>-0.327226739022899</v>
+      </c>
+      <c r="B5">
+        <v>-78.200883849963802</v>
+      </c>
+      <c r="C5">
+        <v>4109.3833473819404</v>
+      </c>
+      <c r="D5">
+        <v>25.870513211373499</v>
+      </c>
+      <c r="E5" s="5">
+        <v>29</v>
+      </c>
+      <c r="F5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H5" s="3"/>
+      <c r="I5" t="s">
+        <v>10</v>
+      </c>
+      <c r="J5" t="s">
+        <v>10</v>
+      </c>
+      <c r="O5" t="s">
+        <v>11</v>
+      </c>
+      <c r="P5">
+        <v>4106.109375</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A6">
+        <v>-0.32723973902289899</v>
+      </c>
+      <c r="B6">
+        <v>-78.200874346437004</v>
+      </c>
+      <c r="C6">
+        <v>4109.2851070432298</v>
+      </c>
+      <c r="D6">
+        <v>27.654686536295799</v>
+      </c>
+      <c r="E6" s="5">
+        <v>31</v>
+      </c>
+      <c r="F6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H6" s="3"/>
+      <c r="I6" t="s">
+        <v>10</v>
+      </c>
+      <c r="J6" t="s">
+        <v>10</v>
+      </c>
+      <c r="O6" t="s">
+        <v>11</v>
+      </c>
+      <c r="P6">
+        <v>4105.8173828125</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A7">
+        <v>-0.32734363902289898</v>
+      </c>
+      <c r="B7">
+        <v>-78.200764054001496</v>
+      </c>
+      <c r="C7">
+        <v>4107.6678583000303</v>
+      </c>
+      <c r="D7">
+        <v>44.6043331230577</v>
+      </c>
+      <c r="E7" s="5">
+        <v>50</v>
+      </c>
+      <c r="F7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7" t="s">
+        <v>10</v>
+      </c>
+      <c r="H7" s="3"/>
+      <c r="I7" t="s">
+        <v>10</v>
+      </c>
+      <c r="J7" t="s">
+        <v>10</v>
+      </c>
+      <c r="P7">
+        <v>4104.736328125</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A8">
+        <v>-0.32733903902289901</v>
+      </c>
+      <c r="B8">
+        <v>-78.2007707147242</v>
+      </c>
+      <c r="C8">
+        <v>4107.7924576281202</v>
+      </c>
+      <c r="D8">
+        <v>43.703230106822303</v>
+      </c>
+      <c r="H8" s="4">
+        <v>44376</v>
+      </c>
+      <c r="I8">
+        <v>0.90500000000000003</v>
+      </c>
+      <c r="J8">
+        <v>4965.0874679999997</v>
+      </c>
+      <c r="K8">
+        <v>7.1980000000000004</v>
+      </c>
+      <c r="L8">
+        <v>627.08240000000001</v>
+      </c>
+      <c r="M8" t="s">
+        <v>20</v>
+      </c>
+      <c r="N8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A9">
+        <v>-0.32722793902289898</v>
+      </c>
+      <c r="B9">
+        <v>-78.2008829972131</v>
+      </c>
+      <c r="C9">
+        <v>4109.3746016283703</v>
+      </c>
+      <c r="D9">
+        <v>26.028797472404602</v>
+      </c>
+      <c r="H9" s="4">
+        <v>44377</v>
+      </c>
+      <c r="I9">
+        <v>0.46500000000000002</v>
+      </c>
+      <c r="J9">
+        <v>2015.4536559999999</v>
+      </c>
+      <c r="K9">
+        <v>6.8090000000000002</v>
+      </c>
+      <c r="L9">
+        <v>626.23339999999996</v>
+      </c>
+      <c r="M9" t="s">
+        <v>20</v>
+      </c>
+      <c r="N9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A10">
+        <v>-0.32717543902289897</v>
+      </c>
+      <c r="B10">
+        <v>-78.200917287477907</v>
+      </c>
+      <c r="C10">
+        <v>4109.7416985772397</v>
+      </c>
+      <c r="D10">
+        <v>19.047127018458699</v>
+      </c>
+      <c r="H10" s="4">
+        <v>44377</v>
+      </c>
+      <c r="I10">
+        <v>0.255</v>
+      </c>
+      <c r="J10">
+        <v>1334.1187399999999</v>
+      </c>
+      <c r="K10">
+        <v>6.7679999999999998</v>
+      </c>
+      <c r="L10">
+        <v>626.18640000000005</v>
+      </c>
+      <c r="M10" t="s">
+        <v>20</v>
+      </c>
+      <c r="N10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A11">
+        <v>-0.32711823902289899</v>
+      </c>
+      <c r="B11">
+        <v>-78.200954072161196</v>
+      </c>
+      <c r="C11">
+        <v>4110.1707625115396</v>
+      </c>
+      <c r="D11">
+        <v>11.475627166117899</v>
+      </c>
+      <c r="H11" s="4">
+        <v>44376</v>
+      </c>
+      <c r="I11">
+        <v>0.105</v>
+      </c>
+      <c r="J11">
+        <v>2074.6903579999998</v>
+      </c>
+      <c r="K11">
+        <v>7.1959999999999997</v>
+      </c>
+      <c r="L11">
+        <v>627.11239999999998</v>
+      </c>
+      <c r="M11" t="s">
+        <v>20</v>
+      </c>
+      <c r="N11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A12">
+        <v>-0.32711163902289903</v>
+      </c>
+      <c r="B12">
+        <v>-78.200958742254102</v>
+      </c>
+      <c r="C12">
+        <v>4110.2459241233901</v>
+      </c>
+      <c r="D12">
+        <v>10.5755891925486</v>
+      </c>
+      <c r="H12" s="4">
+        <v>44377</v>
+      </c>
+      <c r="I12">
+        <v>0.105</v>
+      </c>
+      <c r="J12">
+        <v>1834.5891389999999</v>
+      </c>
+      <c r="K12">
+        <v>6.8230000000000004</v>
+      </c>
+      <c r="L12">
+        <v>626.09040000000005</v>
+      </c>
+      <c r="M12" t="s">
+        <v>20</v>
+      </c>
+      <c r="N12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A13">
+        <v>-0.32704063902289898</v>
+      </c>
+      <c r="B13">
+        <v>-78.201021593015099</v>
+      </c>
+      <c r="C13">
+        <v>4111.5066070908297</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="H13" s="4">
+        <v>44376</v>
+      </c>
+      <c r="I13">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="J13">
+        <v>6479.9494100000002</v>
+      </c>
+      <c r="K13">
+        <v>7.1959999999999997</v>
+      </c>
+      <c r="L13">
+        <v>627.14239999999995</v>
+      </c>
+      <c r="M13" t="s">
+        <v>20</v>
+      </c>
+      <c r="N13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A14">
+        <v>-0.32704063902289898</v>
+      </c>
+      <c r="B14">
+        <v>-78.201021593015099</v>
+      </c>
+      <c r="C14">
+        <v>4111.5066070908297</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="H14" s="4">
+        <v>44377</v>
+      </c>
+      <c r="I14">
+        <v>0.155</v>
+      </c>
+      <c r="J14">
+        <v>1826.5340630000001</v>
+      </c>
+      <c r="K14">
+        <v>6.8259999999999996</v>
+      </c>
+      <c r="L14">
+        <v>626.14739999999995</v>
+      </c>
+      <c r="M14" t="s">
+        <v>20</v>
+      </c>
+      <c r="N14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>